<commit_message>
Started to add something on COIs
</commit_message>
<xml_diff>
--- a/inputs/AddictO_Research_activity_Defs.xlsx
+++ b/inputs/AddictO_Research_activity_Defs.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1975" uniqueCount="761">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1980" uniqueCount="766">
   <si>
     <t>ID</t>
   </si>
@@ -2311,6 +2311,21 @@
   </si>
   <si>
     <t>Double-blind study</t>
+  </si>
+  <si>
+    <t>Report; IAO:0000088</t>
+  </si>
+  <si>
+    <t>A report that provides information about a publication author's interests that could influence how readers understand the publication.</t>
+  </si>
+  <si>
+    <t>The time frame for this reporting is that of the work itself, from the initial conception and planning to the present. The requested information is about resources that the author received, either directly or indirectly (via their institution), to enable them to complete the work. This is not present if the author did the work without receiving any financial support from any third party -- that is, the work was supported by funds from the same institution that pays the person's salary and that institution did not receive third-party funds with which to pay them. If the author or their institution received funds from a third party to support the work, such as a government granting agency, charitable foundation or commercial sponsor, there is a competing interest</t>
+  </si>
+  <si>
+    <t>Potential conflict of interest</t>
+  </si>
+  <si>
+    <t>Disclosure of potential conflict of interest</t>
   </si>
 </sst>
 </file>
@@ -2837,11 +2852,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S548"/>
+  <dimension ref="A1:S546"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A511" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G521" sqref="G521"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A523" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B525" sqref="B525"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2855,7 +2870,7 @@
     <col min="7" max="7" width="35.42578125" style="12" customWidth="1"/>
     <col min="8" max="8" width="48.28515625" style="12" customWidth="1"/>
     <col min="9" max="9" width="23.42578125" style="12" customWidth="1"/>
-    <col min="10" max="10" width="29.7109375" style="12" customWidth="1"/>
+    <col min="10" max="10" width="82.28515625" style="12" customWidth="1"/>
     <col min="11" max="11" width="44.140625" style="12" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="12"/>
     <col min="13" max="13" width="18.42578125" style="12" customWidth="1"/>
@@ -10682,27 +10697,33 @@
       </c>
       <c r="S523" s="13"/>
     </row>
-    <row r="524" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B524" s="14"/>
+    <row r="524" spans="1:19" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B524" s="14" t="s">
+        <v>765</v>
+      </c>
+      <c r="C524" s="11" t="s">
+        <v>762</v>
+      </c>
+      <c r="D524" s="11" t="s">
+        <v>761</v>
+      </c>
+      <c r="E524" s="11" t="s">
+        <v>61</v>
+      </c>
       <c r="P524" s="11" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="525" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B525" s="14"/>
-      <c r="F525" s="12"/>
-      <c r="G525" s="12"/>
-      <c r="H525" s="14"/>
-      <c r="I525" s="12"/>
-      <c r="J525" s="12"/>
-      <c r="K525" s="12"/>
-      <c r="L525" s="12">
-        <v>1</v>
-      </c>
-      <c r="M525" s="12"/>
-      <c r="N525" s="12"/>
-      <c r="O525" s="12"/>
-      <c r="P525" s="12"/>
+    <row r="525" spans="1:19" s="11" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B525" s="14" t="s">
+        <v>764</v>
+      </c>
+      <c r="J525" s="11" t="s">
+        <v>763</v>
+      </c>
+      <c r="P525" s="11" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="526" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B526" s="14"/>
@@ -10712,9 +10733,19 @@
     </row>
     <row r="527" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B527" s="14"/>
-      <c r="P527" s="11" t="s">
-        <v>121</v>
-      </c>
+      <c r="D527" s="12"/>
+      <c r="E527" s="12"/>
+      <c r="F527" s="12"/>
+      <c r="G527" s="12"/>
+      <c r="H527" s="12"/>
+      <c r="I527" s="12"/>
+      <c r="J527" s="12"/>
+      <c r="K527" s="12"/>
+      <c r="L527" s="12"/>
+      <c r="M527" s="12"/>
+      <c r="N527" s="12"/>
+      <c r="O527" s="12"/>
+      <c r="P527" s="12"/>
     </row>
     <row r="528" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B528" s="14"/>
@@ -10724,6 +10755,7 @@
     </row>
     <row r="529" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B529" s="14"/>
+      <c r="C529" s="12"/>
       <c r="D529" s="12"/>
       <c r="E529" s="12"/>
       <c r="F529" s="12"/>
@@ -10740,47 +10772,30 @@
     </row>
     <row r="530" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B530" s="14"/>
-      <c r="P530" s="11" t="s">
-        <v>121</v>
-      </c>
+      <c r="C530" s="12"/>
+      <c r="D530" s="12"/>
+      <c r="E530" s="12"/>
+      <c r="F530" s="12"/>
+      <c r="G530" s="12"/>
+      <c r="H530" s="12"/>
+      <c r="I530" s="12"/>
+      <c r="J530" s="12"/>
+      <c r="K530" s="12"/>
+      <c r="L530" s="12"/>
+      <c r="M530" s="12"/>
+      <c r="N530" s="12"/>
+      <c r="O530" s="12"/>
+      <c r="P530" s="12"/>
     </row>
     <row r="531" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B531" s="14"/>
-      <c r="C531" s="12"/>
-      <c r="D531" s="12"/>
-      <c r="E531" s="12"/>
-      <c r="F531" s="12"/>
-      <c r="G531" s="12"/>
-      <c r="H531" s="12"/>
-      <c r="I531" s="12"/>
-      <c r="J531" s="12"/>
-      <c r="K531" s="12"/>
-      <c r="L531" s="12"/>
-      <c r="M531" s="12"/>
-      <c r="N531" s="12"/>
-      <c r="O531" s="12"/>
-      <c r="P531" s="12"/>
+      <c r="Q531" s="12"/>
     </row>
     <row r="532" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B532" s="14"/>
-      <c r="C532" s="12"/>
-      <c r="D532" s="12"/>
-      <c r="E532" s="12"/>
-      <c r="F532" s="12"/>
-      <c r="G532" s="12"/>
-      <c r="H532" s="12"/>
-      <c r="I532" s="12"/>
-      <c r="J532" s="12"/>
-      <c r="K532" s="12"/>
-      <c r="L532" s="12"/>
-      <c r="M532" s="12"/>
-      <c r="N532" s="12"/>
-      <c r="O532" s="12"/>
-      <c r="P532" s="12"/>
     </row>
     <row r="533" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B533" s="14"/>
-      <c r="Q533" s="12"/>
     </row>
     <row r="534" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B534" s="14"/>
@@ -10801,21 +10816,51 @@
       <c r="B539" s="14"/>
     </row>
     <row r="540" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A540" s="14"/>
       <c r="B540" s="14"/>
+      <c r="R540" s="12"/>
     </row>
     <row r="541" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B541" s="14"/>
+      <c r="Q541" s="12"/>
     </row>
     <row r="542" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A542" s="14"/>
       <c r="B542" s="14"/>
-      <c r="R542" s="12"/>
+      <c r="C542" s="12"/>
+      <c r="D542" s="12"/>
+      <c r="E542" s="12"/>
+      <c r="F542" s="12"/>
+      <c r="G542" s="12"/>
+      <c r="H542" s="12"/>
+      <c r="I542" s="12"/>
+      <c r="J542" s="12"/>
+      <c r="K542" s="12"/>
+      <c r="L542" s="12"/>
+      <c r="M542" s="12"/>
+      <c r="N542" s="12"/>
+      <c r="O542" s="12"/>
+      <c r="P542" s="12"/>
     </row>
     <row r="543" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B543" s="14"/>
+      <c r="C543" s="12"/>
+      <c r="D543" s="12"/>
+      <c r="E543" s="12"/>
+      <c r="F543" s="12"/>
+      <c r="G543" s="12"/>
+      <c r="H543" s="12"/>
+      <c r="I543" s="12"/>
+      <c r="J543" s="12"/>
+      <c r="K543" s="12"/>
+      <c r="L543" s="12"/>
+      <c r="M543" s="12"/>
+      <c r="N543" s="12"/>
+      <c r="O543" s="12"/>
+      <c r="P543" s="12"/>
       <c r="Q543" s="12"/>
     </row>
     <row r="544" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A544" s="12"/>
       <c r="B544" s="14"/>
       <c r="C544" s="12"/>
       <c r="D544" s="12"/>
@@ -10831,8 +10876,10 @@
       <c r="N544" s="12"/>
       <c r="O544" s="12"/>
       <c r="P544" s="12"/>
-    </row>
-    <row r="545" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q544" s="12"/>
+      <c r="R544" s="12"/>
+    </row>
+    <row r="545" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B545" s="14"/>
       <c r="C545" s="12"/>
       <c r="D545" s="12"/>
@@ -10850,46 +10897,8 @@
       <c r="P545" s="12"/>
       <c r="Q545" s="12"/>
     </row>
-    <row r="546" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A546" s="12"/>
+    <row r="546" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B546" s="14"/>
-      <c r="C546" s="12"/>
-      <c r="D546" s="12"/>
-      <c r="E546" s="12"/>
-      <c r="F546" s="12"/>
-      <c r="G546" s="12"/>
-      <c r="H546" s="12"/>
-      <c r="I546" s="12"/>
-      <c r="J546" s="12"/>
-      <c r="K546" s="12"/>
-      <c r="L546" s="12"/>
-      <c r="M546" s="12"/>
-      <c r="N546" s="12"/>
-      <c r="O546" s="12"/>
-      <c r="P546" s="12"/>
-      <c r="Q546" s="12"/>
-      <c r="R546" s="12"/>
-    </row>
-    <row r="547" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B547" s="14"/>
-      <c r="C547" s="12"/>
-      <c r="D547" s="12"/>
-      <c r="E547" s="12"/>
-      <c r="F547" s="12"/>
-      <c r="G547" s="12"/>
-      <c r="H547" s="12"/>
-      <c r="I547" s="12"/>
-      <c r="J547" s="12"/>
-      <c r="K547" s="12"/>
-      <c r="L547" s="12"/>
-      <c r="M547" s="12"/>
-      <c r="N547" s="12"/>
-      <c r="O547" s="12"/>
-      <c r="P547" s="12"/>
-      <c r="Q547" s="12"/>
-    </row>
-    <row r="548" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B548" s="14"/>
     </row>
   </sheetData>
   <sortState ref="A2:S2822">

</xml_diff>

<commit_message>
Amendments to competing interest entries
</commit_message>
<xml_diff>
--- a/inputs/AddictO_Research_activity_Defs.xlsx
+++ b/inputs/AddictO_Research_activity_Defs.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2004" uniqueCount="780">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2004" uniqueCount="778">
   <si>
     <t>ID</t>
   </si>
@@ -2328,12 +2328,6 @@
     <t>https://journals.plos.org/plosbiology/s/competing-interests</t>
   </si>
   <si>
-    <t>Researcher attribute</t>
-  </si>
-  <si>
-    <t>An attribute of a researcher that interferes with, or could reasonably be perceived as interfering with, the full and objective enactment of the researcher's role.</t>
-  </si>
-  <si>
     <t>The definition was adapted from the PLOS definition.</t>
   </si>
   <si>
@@ -2343,31 +2337,31 @@
     <t>Potential competing interest</t>
   </si>
   <si>
-    <t>A report that provides information about a researcher's potential competing interest.</t>
-  </si>
-  <si>
-    <t>An attribute of a researcher that could potentially result in a competing interest.</t>
-  </si>
-  <si>
-    <t>Specifically dependent continuant</t>
-  </si>
-  <si>
-    <t>Good practice involves being as inclusive as possible to ensure full transparency and include both financial and non-financial factors that might conceivably influence the conduct, reporting or evaluation of research whether or not it actually does so.</t>
-  </si>
-  <si>
     <t>Financial potential competing interest</t>
   </si>
   <si>
-    <t>A potential competing interest that involves the potential for personal financial gain or loss resulting from enactment of the researcher's role.</t>
-  </si>
-  <si>
-    <t>Competing interests carry no implication of wrong-doing and are often unavoidable in research. However, they must be fully disclosed to enable users of research and research reports to make an informed judgement about the potential for bias.</t>
-  </si>
-  <si>
-    <t>This includes: 1) financial potential competing interest as well as 2) potentially being personally affected by, 3) having close friends, colleagues or relations who may be affected by, 4) having strong values relating to, 5) acting as an advisor to an organisation that may be affected by, and 6) being a member of a lobby group or pressure group relating to, the reported outcome of the research.</t>
-  </si>
-  <si>
-    <t>This includes: 1) ownership of stocks or shares, 2) employment in an organisation, 3) providing paid consultancy to an organisation, 4) being a director of a company, 5) receiving any kind of funding or tangible benefit (e.g. research grant, travel funding, hospitality, gift) from an organisation, 6) ownership of, or pending application for, a patent, and 7) seeking funding from an organisation, that may be affected by the reported outcome of the research. It also includes all of the above that relate to an intimate partner. Organisation includes commercial organisation, government agency, and charity.</t>
+    <t>An attribute of a person that could be a competing interest.</t>
+  </si>
+  <si>
+    <t>A potential competing interest that involves the potential for personal financial gain or loss resulting from enactment of the professional role.</t>
+  </si>
+  <si>
+    <t>Good practice involves being as inclusive as possible to ensure full transparency and include both financial and non-financial attributes that might conceivably influence the conduct, reporting or evaluation of research whether or not it actually does so.</t>
+  </si>
+  <si>
+    <t>Competing interests carry no implication of wrong-doing and are often unavoidable. However, they must be fully disclosed to enable stakeholders to make an informed judgement about the potential for bias.</t>
+  </si>
+  <si>
+    <t>This includes: 1) financial potential competing interest as well as 2) potentially being personally affected by, 3) having close friends, colleagues or relations who may be affected by, 4) having strong values relating to, 5) acting as an advisor to an organisation that may be affected by, and 6) being a member of a lobby group or pressure group relating to, the conduct of the professional role.</t>
+  </si>
+  <si>
+    <t>This includes: 1) ownership of stocks or shares, 2) employment in an organisation, 3) providing paid consultancy to an organisation, 4) being a director of a company, 5) receiving any kind of funding or tangible benefit (e.g. research grant, travel funding, hospitality, gift) from an organisation, 6) ownership of, or pending application for, a patent, and 7) seeking funding from an organisation, that may be affected by the enactment of the professional role. It also includes all of the above that relate to an intimate partner. Organisation includes commercial organisation, government agency, and charity.</t>
+  </si>
+  <si>
+    <t>A report that provides information about a person's potential competing interest.</t>
+  </si>
+  <si>
+    <t>An attribute of a person that interferes with the full and objective enactment of a professional role.</t>
   </si>
 </sst>
 </file>
@@ -2629,7 +2623,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2930,7 +2924,7 @@
   <dimension ref="A1:S546"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C514" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C520" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="C527" sqref="C527"/>
@@ -10782,10 +10776,10 @@
     </row>
     <row r="524" spans="1:19" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B524" s="25" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="C524" s="24" t="s">
-        <v>771</v>
+        <v>776</v>
       </c>
       <c r="D524" s="24" t="s">
         <v>761</v>
@@ -10797,7 +10791,7 @@
         <v>712</v>
       </c>
       <c r="J524" s="24" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="P524" s="24" t="s">
         <v>121</v>
@@ -10808,13 +10802,13 @@
         <v>764</v>
       </c>
       <c r="C525" s="24" t="s">
-        <v>767</v>
+        <v>777</v>
       </c>
       <c r="D525" s="24" t="s">
-        <v>766</v>
+        <v>70</v>
       </c>
       <c r="E525" s="24" t="s">
-        <v>773</v>
+        <v>70</v>
       </c>
       <c r="F525" s="24" t="s">
         <v>712</v>
@@ -10823,10 +10817,10 @@
         <v>765</v>
       </c>
       <c r="H525" s="24" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="J525" s="24" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="P525" s="24" t="s">
         <v>121</v>
@@ -10834,25 +10828,25 @@
     </row>
     <row r="526" spans="1:19" s="24" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="B526" s="25" t="s">
+        <v>768</v>
+      </c>
+      <c r="C526" s="24" t="s">
         <v>770</v>
       </c>
-      <c r="C526" s="24" t="s">
-        <v>772</v>
-      </c>
       <c r="D526" s="24" t="s">
-        <v>766</v>
+        <v>70</v>
       </c>
       <c r="E526" s="24" t="s">
-        <v>773</v>
+        <v>70</v>
       </c>
       <c r="F526" s="24" t="s">
         <v>712</v>
       </c>
       <c r="H526" s="24" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="J526" s="24" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="P526" s="24" t="s">
         <v>121</v>
@@ -10860,27 +10854,27 @@
     </row>
     <row r="527" spans="1:19" s="24" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="B527" s="25" t="s">
-        <v>775</v>
+        <v>769</v>
       </c>
       <c r="C527" s="24" t="s">
-        <v>776</v>
+        <v>771</v>
       </c>
       <c r="D527" s="27" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="E527" s="24" t="s">
-        <v>773</v>
+        <v>70</v>
       </c>
       <c r="F527" s="24" t="s">
         <v>712</v>
       </c>
       <c r="G527" s="27"/>
       <c r="H527" s="24" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="I527" s="27"/>
       <c r="J527" s="27" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="K527" s="27"/>
       <c r="L527" s="27"/>

</xml_diff>